<commit_message>
Renouveau DonneeTest et Changement commentaire
</commit_message>
<xml_diff>
--- a/DonneeTest_FFD1.xlsx
+++ b/DonneeTest_FFD1.xlsx
@@ -369,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -403,25 +403,25 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B2">
-        <v>98</v>
+        <v>199</v>
       </c>
       <c r="C2">
-        <v>48</v>
+        <v>188</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F2">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
       <c r="H2">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -429,307 +429,367 @@
     </row>
     <row r="3" spans="1:9">
       <c r="C3">
-        <v>58</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="C4">
-        <v>31</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="C5">
-        <v>46</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="C6">
-        <v>78</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="C7">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="C8">
-        <v>55</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="C9">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="C10">
-        <v>89</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="C11">
-        <v>78</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="C12">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="C13">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="C14">
-        <v>61</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="C15">
-        <v>29</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="C16">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19">
-        <v>28</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20">
-        <v>72</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21">
-        <v>96</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22">
-        <v>47</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24">
-        <v>3</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25">
-        <v>95</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27">
-        <v>36</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="3:3">
       <c r="C28">
-        <v>58</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="3:3">
       <c r="C29">
-        <v>8</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30">
-        <v>16</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31">
-        <v>45</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="3:3">
       <c r="C32">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="3:3">
       <c r="C33">
-        <v>80</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34">
-        <v>10</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36">
-        <v>13</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="3:3">
       <c r="C37">
-        <v>98</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="3:3">
       <c r="C38">
-        <v>58</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="3:3">
       <c r="C39">
-        <v>17</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="3:3">
       <c r="C40">
-        <v>46</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="3:3">
       <c r="C41">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="3:3">
       <c r="C42">
-        <v>1</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="3:3">
       <c r="C43">
-        <v>37</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="3:3">
       <c r="C44">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="3:3">
       <c r="C45">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="3:3">
       <c r="C46">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="3:3">
       <c r="C47">
-        <v>51</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="3:3">
       <c r="C48">
-        <v>30</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51">
-        <v>96</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52">
-        <v>4</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="3:3">
       <c r="C53">
-        <v>21</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="3:3">
       <c r="C54">
-        <v>44</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="3:3">
       <c r="C55">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="3:3">
       <c r="C56">
-        <v>31</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="3:3">
       <c r="C57">
-        <v>22</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="3:3">
       <c r="C58">
-        <v>64</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="3:3">
       <c r="C59">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="3:3">
       <c r="C60">
-        <v>12</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="3:3">
       <c r="C61">
-        <v>66</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="3:3">
       <c r="C62">
-        <v>95</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="3:3">
       <c r="C63">
-        <v>27</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3">
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3">
+      <c r="C70">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3">
+      <c r="C71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>